<commit_message>
refactored projected production to use ghg_s1s2 values and benchmarks
</commit_message>
<xml_diff>
--- a/test/inputs/test_data_sector.xlsx
+++ b/test/inputs/test_data_sector.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jurj\Smartgit\ITR\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorisc\IdeaProjects\ITR\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="projected_ei_in_Wh" sheetId="1" r:id="rId1"/>
     <sheet name="projected_production" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,9 +51,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -87,7 +87,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,17 +371,17 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10:AH15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.81640625" customWidth="1"/>
-    <col min="3" max="34" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="34" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -485,7 +485,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -589,7 +589,7 @@
         <v>0.16000020573809565</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -693,7 +693,7 @@
         <v>0.16000044299039362</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -797,7 +797,7 @@
         <v>0.16001214829601679</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -901,7 +901,7 @@
         <v>3.9901480851305075E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>5.4003654368712638E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1119,19 +1119,19 @@
   <dimension ref="A1:AH7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.08984375" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="34" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="34" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2">
         <v>1.4999999999999999E-2</v>
@@ -1339,7 +1339,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>1.4999999999999999E-2</v>
@@ -1443,7 +1443,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <v>1.4999999999999999E-2</v>
@@ -1547,7 +1547,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>2.4000130214877569E-2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <v>-7.6398544753241149E-2</v>
@@ -1651,7 +1651,7 @@
         <v>1.1912758443362925E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>1.5000548791797463E-2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>-7.6445097814137997E-2</v>
@@ -1755,7 +1755,7 @@
         <v>6.3601028128394965E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>2.0000446929317572E-2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>-7.581010331041782E-2</v>

</xml_diff>